<commit_message>
financial analysis assignment beta
</commit_message>
<xml_diff>
--- a/semester C/Financial_Analysis/ALPHA_Financials_2023_2024.xlsx
+++ b/semester C/Financial_Analysis/ALPHA_Financials_2023_2024.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>Κατάσταση Αποτελεσμάτων Χρήσης</t>
   </si>
@@ -201,25 +201,49 @@
     <t>Column4</t>
   </si>
   <si>
+    <t>P1</t>
+  </si>
+  <si>
     <t>Ratio / Parameter</t>
   </si>
   <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Div1</t>
+  </si>
+  <si>
     <t>--- Valuation Parameters ---</t>
   </si>
   <si>
+    <t>g</t>
+  </si>
+  <si>
     <t>Share Price (€)</t>
   </si>
   <si>
     <t>τιμή ανά μετοχή</t>
   </si>
   <si>
+    <t>P0 (Div1 + P1)/(1+r)</t>
+  </si>
+  <si>
     <t>Shares Outstanding (Ε000)</t>
   </si>
   <si>
+    <t>P0 (10 years)</t>
+  </si>
+  <si>
     <t>Market Cap (€000)</t>
   </si>
   <si>
+    <t>P0 (10 years) 0 P1</t>
+  </si>
+  <si>
     <t>Net Debt (€000)</t>
+  </si>
+  <si>
+    <t>P0 (infinite) ?</t>
   </si>
   <si>
     <t>DPS (€)</t>
@@ -388,13 +412,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +437,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -576,7 +607,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,13 +622,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,12 +784,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -782,12 +825,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -904,124 +962,118 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1030,86 +1082,97 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1118,19 +1181,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1710,8 +1773,8 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.0925925925926" style="11" customWidth="1"/>
-    <col min="3" max="5" width="10.3611111111111" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.0925925925926" style="16" customWidth="1"/>
+    <col min="3" max="5" width="10.3611111111111" style="17" customWidth="1"/>
     <col min="6" max="6" width="1.72222222222222" style="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="10" width="7.90740740740741" customWidth="1"/>
@@ -1723,1626 +1786,1626 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.6" spans="1:18">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
     </row>
     <row r="2" ht="14" customHeight="1" spans="1:18">
-      <c r="A2" s="13"/>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="17" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="17" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" ht="14" customHeight="1" spans="1:18">
-      <c r="A3" s="13"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="26">
         <v>22000</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="26">
         <v>24000</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="26">
         <v>26500</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="28">
         <v>17000</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="28">
         <v>18000</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="28">
         <v>19000</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="28" t="s">
+      <c r="K3" s="18"/>
+      <c r="L3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="38">
+      <c r="N3" s="43">
         <f>D11</f>
         <v>2652</v>
       </c>
-      <c r="O3" s="38">
+      <c r="O3" s="43">
         <f>E11</f>
         <v>3315</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
     </row>
     <row r="4" ht="14" customHeight="1" spans="1:18">
-      <c r="A4" s="13"/>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="26">
         <v>15400</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="26">
         <v>16800</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="26">
         <v>18200</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="28">
         <v>0</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="28">
         <v>800</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="28">
         <v>1700</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="28" t="s">
+      <c r="K4" s="18"/>
+      <c r="L4" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="38">
+      <c r="N4" s="43">
         <f>I4-H4</f>
         <v>800</v>
       </c>
-      <c r="O4" s="38">
+      <c r="O4" s="43">
         <f>J4-I4</f>
         <v>900</v>
       </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
     </row>
     <row r="5" ht="14" customHeight="1" spans="1:18">
-      <c r="A5" s="13"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="30">
         <f>C3-C4</f>
         <v>6600</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="30">
         <f t="shared" ref="D5:E5" si="0">D3-D4</f>
         <v>7200</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="30">
         <f t="shared" si="0"/>
         <v>8300</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="31">
         <f>H3-H4</f>
         <v>17000</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="31">
         <f>I3-I4</f>
         <v>17200</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="31">
         <f>J3-J4</f>
         <v>17300</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="38">
+      <c r="N5" s="43">
         <f>-(I6-H6)</f>
         <v>-500</v>
       </c>
-      <c r="O5" s="38">
+      <c r="O5" s="43">
         <f>-(J6-I6)</f>
         <v>-500</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
     </row>
     <row r="6" ht="14" customHeight="1" spans="1:18">
-      <c r="A6" s="13"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="26">
         <v>3000</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="26">
         <v>3200</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="26">
         <v>3400</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="27" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="31">
         <v>4500</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="31">
         <v>5000</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="31">
         <v>5500</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="28" t="s">
+      <c r="K6" s="18"/>
+      <c r="L6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="38">
+      <c r="N6" s="43">
         <f>-(I7-H7)</f>
         <v>-300</v>
       </c>
-      <c r="O6" s="38">
+      <c r="O6" s="43">
         <f>-(J7-I7)</f>
         <v>-300</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
     </row>
     <row r="7" ht="14" customHeight="1" spans="1:18">
-      <c r="A7" s="13"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="30">
         <f>C5-C6</f>
         <v>3600</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="30">
         <f t="shared" ref="D7:E7" si="1">D5-D6</f>
         <v>4000</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="30">
         <f t="shared" si="1"/>
         <v>4900</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="28">
         <v>3700</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="28">
         <v>4000</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="28">
         <v>4300</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="28" t="s">
+      <c r="K7" s="18"/>
+      <c r="L7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="38">
+      <c r="N7" s="43">
         <f>(I12-H12)</f>
         <v>300</v>
       </c>
-      <c r="O7" s="38">
+      <c r="O7" s="43">
         <f>(J12-I12)</f>
         <v>200</v>
       </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
     </row>
     <row r="8" ht="14" customHeight="1" spans="1:18">
-      <c r="A8" s="13"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="26">
         <v>500</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="26">
         <v>600</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="26">
         <v>650</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="27" t="s">
+      <c r="F8" s="18"/>
+      <c r="G8" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="31">
         <v>1500</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="31">
         <f>H8+N13</f>
         <v>3523.8</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="31">
         <f>I8+O13</f>
         <v>5478.55</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="28" t="s">
+      <c r="K8" s="18"/>
+      <c r="L8" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="38">
+      <c r="N8" s="43">
         <f>SUM(N3:N7)</f>
         <v>2952</v>
       </c>
-      <c r="O8" s="38">
+      <c r="O8" s="43">
         <f>SUM(O3:O7)</f>
         <v>3615</v>
       </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
     </row>
     <row r="9" ht="14" customHeight="1" spans="1:18">
-      <c r="A9" s="13"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="30">
         <f>C7-C8</f>
         <v>3100</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="30">
         <f t="shared" ref="D9:E9" si="2">D7-D8</f>
         <v>3400</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="30">
         <f t="shared" si="2"/>
         <v>4250</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="18"/>
+      <c r="G9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="34">
         <f>H5+H6+H7+H8</f>
         <v>26700</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="34">
         <f>I5+I6+I7+I8</f>
         <v>29723.8</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="34">
         <f>J5+J6+J7+J8</f>
         <v>32578.55</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="28" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="38">
+      <c r="N9" s="43">
         <f>-(I3-H3)</f>
         <v>-1000</v>
       </c>
-      <c r="O9" s="38">
+      <c r="O9" s="43">
         <f>-(J3-I3)</f>
         <v>-1000</v>
       </c>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
     </row>
     <row r="10" ht="14" customHeight="1" spans="1:18">
-      <c r="A10" s="13"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="26">
         <f>C9*0.22</f>
         <v>682</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="26">
         <f t="shared" ref="D10:E10" si="3">D9*0.22</f>
         <v>748</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="26">
         <f t="shared" si="3"/>
         <v>935</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="18"/>
+      <c r="G10" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="34">
         <v>14000</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="34">
         <f>H10+D15</f>
         <v>15723.8</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="34">
         <f>I10+E15</f>
         <v>17878.55</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="28" t="s">
+      <c r="K10" s="18"/>
+      <c r="L10" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="27" t="s">
+      <c r="M10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="38">
+      <c r="N10" s="43">
         <f>(I11-H11)</f>
         <v>1000</v>
       </c>
-      <c r="O10" s="38">
+      <c r="O10" s="43">
         <f>(J11-I11)</f>
         <v>500</v>
       </c>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
     </row>
     <row r="11" ht="14" customHeight="1" spans="1:18">
-      <c r="A11" s="13"/>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="30">
         <f>C9-C10</f>
         <v>2418</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="30">
         <f t="shared" ref="D11:E11" si="4">D9-D10</f>
         <v>2652</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="30">
         <f t="shared" si="4"/>
         <v>3315</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="22" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="28">
         <v>7000</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="28">
         <v>8000</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="28">
         <v>8500</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27" t="s">
+      <c r="K11" s="18"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="38">
+      <c r="N11" s="43">
         <f>-D14</f>
         <v>-928.2</v>
       </c>
-      <c r="O11" s="38">
+      <c r="O11" s="43">
         <f>-E14</f>
         <v>-1160.25</v>
       </c>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
     </row>
     <row r="12" ht="14" customHeight="1" spans="1:18">
-      <c r="A12" s="13"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="26">
         <f>H4</f>
         <v>0</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="26">
         <f>I4-H4</f>
         <v>800</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="26">
         <f>J4-I4</f>
         <v>900</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="22" t="s">
+      <c r="F12" s="18"/>
+      <c r="G12" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="28">
         <v>5700</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="28">
         <v>6000</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="28">
         <v>6200</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="28" t="s">
+      <c r="K12" s="18"/>
+      <c r="L12" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="M12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="N12" s="38">
+      <c r="N12" s="43">
         <f>N10+N11</f>
         <v>71.8000000000001</v>
       </c>
-      <c r="O12" s="38">
+      <c r="O12" s="43">
         <f>O10+O11</f>
         <v>-660.25</v>
       </c>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
     </row>
     <row r="13" ht="14" customHeight="1" spans="1:18">
-      <c r="A13" s="13"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="30">
         <f>C7+C12</f>
         <v>3600</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="30">
         <f>D7+D12</f>
         <v>4800</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="30">
         <f>E7+E12</f>
         <v>5800</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="28" t="s">
+      <c r="F13" s="18"/>
+      <c r="G13" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="34">
         <f>H10+H11+H12</f>
         <v>26700</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="34">
         <f t="shared" ref="I13:J13" si="5">I10+I11+I12</f>
         <v>29723.8</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="34">
         <f t="shared" si="5"/>
         <v>32578.55</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="28" t="s">
+      <c r="K13" s="18"/>
+      <c r="L13" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="27" t="s">
+      <c r="M13" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="N13" s="38">
+      <c r="N13" s="43">
         <f>N8+N9+N12</f>
         <v>2023.8</v>
       </c>
-      <c r="O13" s="38">
+      <c r="O13" s="43">
         <f>O8+O9+O12</f>
         <v>1954.75</v>
       </c>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
     </row>
     <row r="14" ht="14" customHeight="1" spans="1:18">
-      <c r="A14" s="13"/>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="36">
         <f>0.35*C11</f>
         <v>846.3</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="36">
         <f t="shared" ref="D14:E14" si="6">0.35*D11</f>
         <v>928.2</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="36">
         <f t="shared" si="6"/>
         <v>1160.25</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="28" t="s">
+      <c r="F14" s="18"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="39">
+      <c r="M14" s="44">
         <v>1500</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="45">
         <f>H8</f>
         <v>1500</v>
       </c>
-      <c r="O14" s="40">
+      <c r="O14" s="45">
         <f>I8</f>
         <v>3523.8</v>
       </c>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
     </row>
     <row r="15" ht="14" customHeight="1" spans="1:18">
-      <c r="A15" s="13"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="18"/>
+      <c r="B15" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="36">
         <f>C11-C14</f>
         <v>1571.7</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="36">
         <f t="shared" ref="D15:E15" si="7">D11-D14</f>
         <v>1723.8</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="36">
         <f t="shared" si="7"/>
         <v>2154.75</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="28" t="s">
+      <c r="F15" s="18"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="M15" s="27" t="s">
+      <c r="M15" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="38">
+      <c r="N15" s="43">
         <f>N13+N14</f>
         <v>3523.8</v>
       </c>
-      <c r="O15" s="38">
+      <c r="O15" s="43">
         <f>O13+O14</f>
         <v>5478.55</v>
       </c>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A16" s="13"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A17" s="13"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A18" s="13"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A19" s="13"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A20" s="13"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A21" s="13"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A22" s="13"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A23" s="13"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A24" s="13"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A25" s="13"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A26" s="13"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A27" s="13"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A28" s="13"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A29" s="13"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A30" s="13"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="15.6" spans="1:18">
-      <c r="A31" s="13"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
     </row>
     <row r="32" s="1" customFormat="1" spans="2:5">
-      <c r="B32" s="35"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
     </row>
     <row r="33" s="1" customFormat="1" spans="2:5">
-      <c r="B33" s="35"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
     </row>
     <row r="34" s="1" customFormat="1" spans="2:5">
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
     </row>
     <row r="35" s="1" customFormat="1" spans="2:5">
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
     </row>
     <row r="36" s="1" customFormat="1" spans="2:5">
-      <c r="B36" s="35"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
     </row>
     <row r="37" s="1" customFormat="1" spans="2:5">
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
     </row>
     <row r="38" s="1" customFormat="1" spans="2:5">
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
     </row>
     <row r="39" s="1" customFormat="1" spans="2:5">
-      <c r="B39" s="35"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
     </row>
     <row r="40" s="1" customFormat="1" spans="2:5">
-      <c r="B40" s="35"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
     </row>
     <row r="41" s="1" customFormat="1" spans="2:5">
-      <c r="B41" s="35"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
     </row>
     <row r="42" s="1" customFormat="1" spans="2:5">
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
     </row>
     <row r="43" s="1" customFormat="1" spans="2:5">
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
     </row>
     <row r="44" s="1" customFormat="1" spans="2:5">
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
     </row>
     <row r="45" s="1" customFormat="1" spans="2:5">
-      <c r="B45" s="35"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
     </row>
     <row r="46" s="1" customFormat="1" spans="2:5">
-      <c r="B46" s="35"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
     </row>
     <row r="47" s="1" customFormat="1" spans="2:5">
-      <c r="B47" s="35"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
     </row>
     <row r="48" s="1" customFormat="1" spans="2:5">
-      <c r="B48" s="35"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
     </row>
     <row r="49" s="1" customFormat="1" spans="2:5">
-      <c r="B49" s="35"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
     </row>
     <row r="50" s="1" customFormat="1" spans="2:5">
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
     </row>
     <row r="51" s="1" customFormat="1" spans="2:5">
-      <c r="B51" s="35"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="2:5">
-      <c r="B52" s="35"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
     </row>
     <row r="53" s="1" customFormat="1" spans="2:5">
-      <c r="B53" s="35"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
     </row>
     <row r="54" s="1" customFormat="1" spans="2:5">
-      <c r="B54" s="35"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
     </row>
     <row r="55" s="1" customFormat="1" spans="2:5">
-      <c r="B55" s="35"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
     </row>
     <row r="56" s="1" customFormat="1" spans="2:5">
-      <c r="B56" s="35"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
     </row>
     <row r="57" s="1" customFormat="1" spans="2:5">
-      <c r="B57" s="35"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
     </row>
     <row r="58" s="1" customFormat="1" spans="2:5">
-      <c r="B58" s="35"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
     </row>
     <row r="59" s="1" customFormat="1" spans="2:5">
-      <c r="B59" s="35"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
     </row>
     <row r="60" s="1" customFormat="1" spans="2:5">
-      <c r="B60" s="35"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
     </row>
     <row r="61" s="1" customFormat="1" spans="2:5">
-      <c r="B61" s="35"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
     </row>
     <row r="62" s="1" customFormat="1" spans="2:5">
-      <c r="B62" s="35"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
     </row>
     <row r="63" s="1" customFormat="1" spans="2:5">
-      <c r="B63" s="35"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="41"/>
     </row>
     <row r="64" s="1" customFormat="1" spans="2:5">
-      <c r="B64" s="35"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="41"/>
+      <c r="E64" s="41"/>
     </row>
     <row r="65" s="1" customFormat="1" spans="2:5">
-      <c r="B65" s="35"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
     </row>
     <row r="66" s="1" customFormat="1" spans="2:5">
-      <c r="B66" s="35"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
     </row>
     <row r="67" s="1" customFormat="1" spans="2:5">
-      <c r="B67" s="35"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="41"/>
     </row>
     <row r="68" s="1" customFormat="1" spans="2:5">
-      <c r="B68" s="35"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
     </row>
     <row r="69" s="1" customFormat="1" spans="2:5">
-      <c r="B69" s="35"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
     </row>
     <row r="70" s="1" customFormat="1" spans="2:5">
-      <c r="B70" s="35"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
     </row>
     <row r="71" s="1" customFormat="1" spans="2:5">
-      <c r="B71" s="35"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="41"/>
     </row>
     <row r="72" s="1" customFormat="1" spans="2:5">
-      <c r="B72" s="35"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
     </row>
     <row r="73" s="1" customFormat="1" spans="2:5">
-      <c r="B73" s="35"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="41"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
     </row>
     <row r="74" s="1" customFormat="1" spans="2:5">
-      <c r="B74" s="35"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="41"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
     </row>
     <row r="75" s="1" customFormat="1" spans="2:5">
-      <c r="B75" s="35"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="41"/>
     </row>
     <row r="76" s="1" customFormat="1" spans="2:5">
-      <c r="B76" s="35"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="41"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
     </row>
     <row r="77" s="1" customFormat="1" spans="2:5">
-      <c r="B77" s="35"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="41"/>
+      <c r="E77" s="41"/>
     </row>
     <row r="78" s="1" customFormat="1" spans="2:5">
-      <c r="B78" s="35"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="41"/>
+      <c r="D78" s="41"/>
+      <c r="E78" s="41"/>
     </row>
     <row r="79" s="1" customFormat="1" spans="2:5">
-      <c r="B79" s="35"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="41"/>
+      <c r="E79" s="41"/>
     </row>
     <row r="80" s="1" customFormat="1" spans="2:5">
-      <c r="B80" s="35"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
+      <c r="B80" s="40"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
     </row>
     <row r="81" s="1" customFormat="1" spans="2:5">
-      <c r="B81" s="35"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
+      <c r="B81" s="40"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="41"/>
     </row>
     <row r="82" s="1" customFormat="1" spans="2:5">
-      <c r="B82" s="35"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
+      <c r="B82" s="40"/>
+      <c r="C82" s="41"/>
+      <c r="D82" s="41"/>
+      <c r="E82" s="41"/>
     </row>
     <row r="83" s="1" customFormat="1" spans="2:5">
-      <c r="B83" s="35"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="41"/>
+      <c r="E83" s="41"/>
     </row>
     <row r="84" s="1" customFormat="1" spans="2:5">
-      <c r="B84" s="35"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="41"/>
+      <c r="D84" s="41"/>
+      <c r="E84" s="41"/>
     </row>
     <row r="85" s="1" customFormat="1" spans="2:5">
-      <c r="B85" s="35"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="41"/>
+      <c r="D85" s="41"/>
+      <c r="E85" s="41"/>
     </row>
     <row r="86" s="1" customFormat="1" spans="2:5">
-      <c r="B86" s="35"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="41"/>
+      <c r="D86" s="41"/>
+      <c r="E86" s="41"/>
     </row>
     <row r="87" s="1" customFormat="1" spans="2:5">
-      <c r="B87" s="35"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+      <c r="E87" s="41"/>
     </row>
     <row r="88" s="1" customFormat="1" spans="2:5">
-      <c r="B88" s="35"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="41"/>
+      <c r="D88" s="41"/>
+      <c r="E88" s="41"/>
     </row>
     <row r="89" s="1" customFormat="1" spans="2:5">
-      <c r="B89" s="35"/>
-      <c r="C89" s="36"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="41"/>
+      <c r="E89" s="41"/>
     </row>
     <row r="90" s="1" customFormat="1" spans="2:5">
-      <c r="B90" s="35"/>
-      <c r="C90" s="36"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="41"/>
+      <c r="D90" s="41"/>
+      <c r="E90" s="41"/>
     </row>
     <row r="91" s="1" customFormat="1" spans="2:5">
-      <c r="B91" s="35"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="41"/>
+      <c r="E91" s="41"/>
     </row>
     <row r="92" s="1" customFormat="1" spans="2:5">
-      <c r="B92" s="35"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
+      <c r="B92" s="40"/>
+      <c r="C92" s="41"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="41"/>
     </row>
     <row r="93" s="1" customFormat="1" spans="2:5">
-      <c r="B93" s="35"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="41"/>
+      <c r="D93" s="41"/>
+      <c r="E93" s="41"/>
     </row>
     <row r="94" s="1" customFormat="1" spans="2:5">
-      <c r="B94" s="35"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="41"/>
+      <c r="D94" s="41"/>
+      <c r="E94" s="41"/>
     </row>
     <row r="95" s="1" customFormat="1" spans="2:5">
-      <c r="B95" s="35"/>
-      <c r="C95" s="36"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="41"/>
+      <c r="D95" s="41"/>
+      <c r="E95" s="41"/>
     </row>
     <row r="96" s="1" customFormat="1" spans="2:5">
-      <c r="B96" s="35"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="36"/>
+      <c r="B96" s="40"/>
+      <c r="C96" s="41"/>
+      <c r="D96" s="41"/>
+      <c r="E96" s="41"/>
     </row>
     <row r="97" s="1" customFormat="1" spans="2:5">
-      <c r="B97" s="35"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
+      <c r="B97" s="40"/>
+      <c r="C97" s="41"/>
+      <c r="D97" s="41"/>
+      <c r="E97" s="41"/>
     </row>
     <row r="98" s="1" customFormat="1" spans="2:5">
-      <c r="B98" s="35"/>
-      <c r="C98" s="36"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
+      <c r="B98" s="40"/>
+      <c r="C98" s="41"/>
+      <c r="D98" s="41"/>
+      <c r="E98" s="41"/>
     </row>
     <row r="99" s="1" customFormat="1" spans="2:5">
-      <c r="B99" s="35"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
+      <c r="B99" s="40"/>
+      <c r="C99" s="41"/>
+      <c r="D99" s="41"/>
+      <c r="E99" s="41"/>
     </row>
     <row r="100" s="1" customFormat="1" spans="2:5">
-      <c r="B100" s="35"/>
-      <c r="C100" s="36"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
+      <c r="B100" s="40"/>
+      <c r="C100" s="41"/>
+      <c r="D100" s="41"/>
+      <c r="E100" s="41"/>
     </row>
     <row r="101" s="1" customFormat="1" spans="2:5">
-      <c r="B101" s="35"/>
-      <c r="C101" s="36"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
+      <c r="B101" s="40"/>
+      <c r="C101" s="41"/>
+      <c r="D101" s="41"/>
+      <c r="E101" s="41"/>
     </row>
     <row r="102" s="1" customFormat="1" spans="2:5">
-      <c r="B102" s="35"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
+      <c r="B102" s="40"/>
+      <c r="C102" s="41"/>
+      <c r="D102" s="41"/>
+      <c r="E102" s="41"/>
     </row>
     <row r="103" s="1" customFormat="1" spans="2:5">
-      <c r="B103" s="35"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
+      <c r="B103" s="40"/>
+      <c r="C103" s="41"/>
+      <c r="D103" s="41"/>
+      <c r="E103" s="41"/>
     </row>
     <row r="104" s="1" customFormat="1" spans="2:5">
-      <c r="B104" s="35"/>
-      <c r="C104" s="36"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
+      <c r="B104" s="40"/>
+      <c r="C104" s="41"/>
+      <c r="D104" s="41"/>
+      <c r="E104" s="41"/>
     </row>
     <row r="105" s="1" customFormat="1" spans="2:5">
-      <c r="B105" s="35"/>
-      <c r="C105" s="36"/>
-      <c r="D105" s="36"/>
-      <c r="E105" s="36"/>
+      <c r="B105" s="40"/>
+      <c r="C105" s="41"/>
+      <c r="D105" s="41"/>
+      <c r="E105" s="41"/>
     </row>
     <row r="106" s="1" customFormat="1" spans="2:5">
-      <c r="B106" s="35"/>
-      <c r="C106" s="36"/>
-      <c r="D106" s="36"/>
-      <c r="E106" s="36"/>
+      <c r="B106" s="40"/>
+      <c r="C106" s="41"/>
+      <c r="D106" s="41"/>
+      <c r="E106" s="41"/>
     </row>
     <row r="107" s="1" customFormat="1" spans="2:5">
-      <c r="B107" s="35"/>
-      <c r="C107" s="36"/>
-      <c r="D107" s="36"/>
-      <c r="E107" s="36"/>
+      <c r="B107" s="40"/>
+      <c r="C107" s="41"/>
+      <c r="D107" s="41"/>
+      <c r="E107" s="41"/>
     </row>
     <row r="108" s="1" customFormat="1" spans="2:5">
-      <c r="B108" s="35"/>
-      <c r="C108" s="36"/>
-      <c r="D108" s="36"/>
-      <c r="E108" s="36"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="41"/>
+      <c r="D108" s="41"/>
+      <c r="E108" s="41"/>
     </row>
     <row r="109" s="1" customFormat="1" spans="2:5">
-      <c r="B109" s="35"/>
-      <c r="C109" s="36"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="36"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="41"/>
+      <c r="D109" s="41"/>
+      <c r="E109" s="41"/>
     </row>
     <row r="110" s="1" customFormat="1" spans="2:5">
-      <c r="B110" s="35"/>
-      <c r="C110" s="36"/>
-      <c r="D110" s="36"/>
-      <c r="E110" s="36"/>
+      <c r="B110" s="40"/>
+      <c r="C110" s="41"/>
+      <c r="D110" s="41"/>
+      <c r="E110" s="41"/>
     </row>
     <row r="111" s="1" customFormat="1" spans="2:5">
-      <c r="B111" s="35"/>
-      <c r="C111" s="36"/>
-      <c r="D111" s="36"/>
-      <c r="E111" s="36"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="41"/>
+      <c r="D111" s="41"/>
+      <c r="E111" s="41"/>
     </row>
     <row r="112" s="1" customFormat="1" spans="2:5">
-      <c r="B112" s="35"/>
-      <c r="C112" s="36"/>
-      <c r="D112" s="36"/>
-      <c r="E112" s="36"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="41"/>
+      <c r="D112" s="41"/>
+      <c r="E112" s="41"/>
     </row>
     <row r="113" s="1" customFormat="1" spans="2:5">
-      <c r="B113" s="35"/>
-      <c r="C113" s="36"/>
-      <c r="D113" s="36"/>
-      <c r="E113" s="36"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="41"/>
+      <c r="D113" s="41"/>
+      <c r="E113" s="41"/>
     </row>
     <row r="114" s="1" customFormat="1" spans="2:5">
-      <c r="B114" s="35"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="41"/>
+      <c r="D114" s="41"/>
+      <c r="E114" s="41"/>
     </row>
     <row r="115" s="1" customFormat="1" spans="2:5">
-      <c r="B115" s="35"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
+      <c r="B115" s="40"/>
+      <c r="C115" s="41"/>
+      <c r="D115" s="41"/>
+      <c r="E115" s="41"/>
     </row>
     <row r="116" s="1" customFormat="1" spans="2:5">
-      <c r="B116" s="35"/>
-      <c r="C116" s="36"/>
-      <c r="D116" s="36"/>
-      <c r="E116" s="36"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="41"/>
+      <c r="D116" s="41"/>
+      <c r="E116" s="41"/>
     </row>
     <row r="117" s="1" customFormat="1" spans="2:5">
-      <c r="B117" s="35"/>
-      <c r="C117" s="36"/>
-      <c r="D117" s="36"/>
-      <c r="E117" s="36"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="41"/>
+      <c r="D117" s="41"/>
+      <c r="E117" s="41"/>
     </row>
     <row r="118" s="1" customFormat="1" spans="2:5">
-      <c r="B118" s="35"/>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
+      <c r="B118" s="40"/>
+      <c r="C118" s="41"/>
+      <c r="D118" s="41"/>
+      <c r="E118" s="41"/>
     </row>
     <row r="119" s="1" customFormat="1" spans="2:5">
-      <c r="B119" s="35"/>
-      <c r="C119" s="36"/>
-      <c r="D119" s="36"/>
-      <c r="E119" s="36"/>
+      <c r="B119" s="40"/>
+      <c r="C119" s="41"/>
+      <c r="D119" s="41"/>
+      <c r="E119" s="41"/>
     </row>
     <row r="120" s="1" customFormat="1" spans="2:5">
-      <c r="B120" s="35"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="36"/>
-      <c r="E120" s="36"/>
+      <c r="B120" s="40"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
+      <c r="E120" s="41"/>
     </row>
     <row r="121" s="1" customFormat="1" spans="2:5">
-      <c r="B121" s="35"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="36"/>
-      <c r="E121" s="36"/>
+      <c r="B121" s="40"/>
+      <c r="C121" s="41"/>
+      <c r="D121" s="41"/>
+      <c r="E121" s="41"/>
     </row>
     <row r="122" s="1" customFormat="1" spans="2:5">
-      <c r="B122" s="35"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="36"/>
-      <c r="E122" s="36"/>
+      <c r="B122" s="40"/>
+      <c r="C122" s="41"/>
+      <c r="D122" s="41"/>
+      <c r="E122" s="41"/>
     </row>
     <row r="123" s="1" customFormat="1" spans="2:5">
-      <c r="B123" s="35"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
-      <c r="E123" s="36"/>
+      <c r="B123" s="40"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="41"/>
+      <c r="E123" s="41"/>
     </row>
     <row r="124" s="1" customFormat="1" spans="2:5">
-      <c r="B124" s="35"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="36"/>
-      <c r="E124" s="36"/>
+      <c r="B124" s="40"/>
+      <c r="C124" s="41"/>
+      <c r="D124" s="41"/>
+      <c r="E124" s="41"/>
     </row>
     <row r="125" s="1" customFormat="1" spans="2:5">
-      <c r="B125" s="35"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="36"/>
-      <c r="E125" s="36"/>
+      <c r="B125" s="40"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="41"/>
+      <c r="E125" s="41"/>
     </row>
     <row r="126" s="1" customFormat="1" spans="2:5">
-      <c r="B126" s="35"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="36"/>
-      <c r="E126" s="36"/>
+      <c r="B126" s="40"/>
+      <c r="C126" s="41"/>
+      <c r="D126" s="41"/>
+      <c r="E126" s="41"/>
     </row>
     <row r="127" s="1" customFormat="1" spans="2:5">
-      <c r="B127" s="35"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
-      <c r="E127" s="36"/>
+      <c r="B127" s="40"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="41"/>
+      <c r="E127" s="41"/>
     </row>
     <row r="128" s="1" customFormat="1" spans="2:5">
-      <c r="B128" s="35"/>
-      <c r="C128" s="36"/>
-      <c r="D128" s="36"/>
-      <c r="E128" s="36"/>
+      <c r="B128" s="40"/>
+      <c r="C128" s="41"/>
+      <c r="D128" s="41"/>
+      <c r="E128" s="41"/>
     </row>
     <row r="129" s="1" customFormat="1" spans="2:5">
-      <c r="B129" s="35"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="36"/>
-      <c r="E129" s="36"/>
+      <c r="B129" s="40"/>
+      <c r="C129" s="41"/>
+      <c r="D129" s="41"/>
+      <c r="E129" s="41"/>
     </row>
     <row r="130" s="1" customFormat="1" spans="2:5">
-      <c r="B130" s="35"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="36"/>
-      <c r="E130" s="36"/>
+      <c r="B130" s="40"/>
+      <c r="C130" s="41"/>
+      <c r="D130" s="41"/>
+      <c r="E130" s="41"/>
     </row>
     <row r="131" s="1" customFormat="1" spans="2:5">
-      <c r="B131" s="35"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
+      <c r="B131" s="40"/>
+      <c r="C131" s="41"/>
+      <c r="D131" s="41"/>
+      <c r="E131" s="41"/>
     </row>
     <row r="132" s="1" customFormat="1" spans="2:5">
-      <c r="B132" s="35"/>
-      <c r="C132" s="36"/>
-      <c r="D132" s="36"/>
-      <c r="E132" s="36"/>
+      <c r="B132" s="40"/>
+      <c r="C132" s="41"/>
+      <c r="D132" s="41"/>
+      <c r="E132" s="41"/>
     </row>
     <row r="133" s="1" customFormat="1" spans="2:5">
-      <c r="B133" s="35"/>
-      <c r="C133" s="36"/>
-      <c r="D133" s="36"/>
-      <c r="E133" s="36"/>
+      <c r="B133" s="40"/>
+      <c r="C133" s="41"/>
+      <c r="D133" s="41"/>
+      <c r="E133" s="41"/>
     </row>
     <row r="134" s="1" customFormat="1" spans="2:5">
-      <c r="B134" s="35"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="36"/>
-      <c r="E134" s="36"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="41"/>
+      <c r="D134" s="41"/>
+      <c r="E134" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3361,24 +3424,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:E813"/>
+  <dimension ref="B1:M813"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.72222222222222" style="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="10.2685185185185" customWidth="1"/>
     <col min="5" max="5" width="49.8888888888889" style="1" customWidth="1"/>
-    <col min="6" max="63" width="8.72222222222222" style="1"/>
+    <col min="6" max="7" width="8.72222222222222" style="1"/>
+    <col min="8" max="8" width="19.1111111111111" style="1" customWidth="1"/>
+    <col min="9" max="63" width="8.72222222222222" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1"/>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:13">
       <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
@@ -3391,10 +3456,28 @@
       <c r="E2" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="H2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="12">
+        <v>5</v>
+      </c>
+      <c r="J2" s="12">
+        <v>5</v>
+      </c>
+      <c r="K2" s="12">
+        <v>5</v>
+      </c>
+      <c r="L2" s="12">
+        <v>5</v>
+      </c>
+      <c r="M2" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2">
         <v>2023</v>
@@ -3402,87 +3485,215 @@
       <c r="D3" s="3">
         <v>2024</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="8:13">
+      <c r="H4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.115</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.115</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.115</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0.115</v>
+      </c>
+      <c r="M4" s="12">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
+        <v>61</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="4">
+        <v>63</v>
+      </c>
+      <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <f>C6</f>
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
+        <v>64</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="12">
+        <v>4.65</v>
+      </c>
+      <c r="J6" s="12">
+        <v>4.65</v>
+      </c>
+      <c r="K6" s="12">
+        <v>4.65</v>
+      </c>
+      <c r="L6" s="12">
+        <v>4.2625</v>
+      </c>
+      <c r="M6" s="12">
+        <v>4.2625</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="5">
+        <v>66</v>
+      </c>
+      <c r="C7" s="6">
         <v>9000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <f t="shared" ref="D7" si="0">C7</f>
         <v>9000</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="H7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="12">
+        <v>5.59090909090909</v>
+      </c>
+      <c r="J7" s="12">
+        <v>5.59090909090909</v>
+      </c>
+      <c r="K7" s="12">
+        <v>5.59090909090909</v>
+      </c>
+      <c r="L7" s="12">
+        <v>5.125</v>
+      </c>
+      <c r="M7" s="12">
+        <v>5.125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="8">
         <f>C6*C7</f>
         <v>45000</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <f>D6*D7</f>
         <v>45000</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="H8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1.04545454545455</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1.04545454545455</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1.04545454545455</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0.958333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="8">
         <f>Balance_Sheet!I11-Balance_Sheet!I8</f>
         <v>4476.2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <f>Balance_Sheet!J11-Balance_Sheet!J8</f>
         <v>3021.45</v>
       </c>
+      <c r="H9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1.15</v>
+      </c>
+      <c r="J9" s="12">
+        <v>2.3</v>
+      </c>
+      <c r="K9" s="12">
+        <v>11.5</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0.575</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0.766666666666667</v>
+      </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="9">
         <f>Balance_Sheet!D14/Ratios_Formulas!C7</f>
         <v>0.103133333333333</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <f>Balance_Sheet!E14/Ratios_Formulas!D7</f>
         <v>0.128916666666667</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="3:3">
-      <c r="C12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C13" s="3">
         <v>2023</v>
@@ -3492,416 +3703,416 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="B14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="8">
         <f>(Balance_Sheet!H6+Balance_Sheet!I6)/2</f>
         <v>4750</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="8">
         <f>(Balance_Sheet!I6+Balance_Sheet!J6)/2</f>
         <v>5250</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="8">
         <f>(Balance_Sheet!H7+Balance_Sheet!I7)/2</f>
         <v>3850</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="8">
         <f>(Balance_Sheet!I7+Balance_Sheet!J7)/2</f>
         <v>4150</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="8">
         <f>(Balance_Sheet!H9+Balance_Sheet!I9)/2</f>
         <v>28211.9</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="8">
         <f>(Balance_Sheet!I8+Balance_Sheet!J8)/2</f>
         <v>4501.175</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="8">
         <f>(Balance_Sheet!H10+Balance_Sheet!I10)/2</f>
         <v>14861.9</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="8">
         <f>(Balance_Sheet!I9+Balance_Sheet!J9)/2</f>
         <v>31151.175</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="8">
         <f>Balance_Sheet!I13</f>
         <v>29723.8</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="8">
         <f>Balance_Sheet!J13</f>
         <v>32578.55</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="8">
         <f>Balance_Sheet!I12</f>
         <v>6000</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="8">
         <f>Balance_Sheet!J12</f>
         <v>6200</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="8">
         <f>Balance_Sheet!I6+Balance_Sheet!I7+Balance_Sheet!I8</f>
         <v>12523.8</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="8">
         <f>Balance_Sheet!J6+Balance_Sheet!J7+Balance_Sheet!J8</f>
         <v>15278.55</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="8">
         <f>C20-C19</f>
         <v>6523.8</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="8">
         <f>D20-D19</f>
         <v>9078.55</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="8">
+      <c r="B22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="9">
         <f>C20/C19</f>
         <v>2.0873</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <f>D20/D19</f>
         <v>2.46428225806452</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="8">
+      <c r="B23" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="9">
         <f>(C20-Balance_Sheet!I6)/Ratios_Formulas!C19</f>
         <v>1.25396666666667</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <f>(D20-Balance_Sheet!J6)/Ratios_Formulas!D19</f>
         <v>1.57718548387097</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="8">
+      <c r="B24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="9">
         <f>Balance_Sheet!I13/Balance_Sheet!I10</f>
         <v>1.89037001233798</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="9">
         <f>Balance_Sheet!J13/Balance_Sheet!J10</f>
         <v>1.82221432946184</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="8">
+      <c r="B25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="9">
         <f>C9/Balance_Sheet!D13</f>
         <v>0.932541666666667</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="9">
         <f>D9/Balance_Sheet!E13</f>
         <v>0.520939655172414</v>
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="9">
+      <c r="B26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="10">
         <f>Balance_Sheet!D11/Balance_Sheet!I10</f>
         <v>0.168661519480024</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="9">
         <f>Balance_Sheet!E11/Balance_Sheet!J10</f>
         <v>0.185417721235783</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="8">
+      <c r="B27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="9">
         <f>Balance_Sheet!D11/Balance_Sheet!I9</f>
         <v>0.0892214319837975</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="10">
         <f>Balance_Sheet!E11/Balance_Sheet!J9</f>
         <v>0.10175406824429</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="9">
+      <c r="B28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="10">
         <f>Balance_Sheet!D13/Balance_Sheet!D3</f>
         <v>0.2</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="10">
         <f>Balance_Sheet!E13/Balance_Sheet!E3</f>
         <v>0.218867924528302</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="9">
+      <c r="B29" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="10">
         <f>Balance_Sheet!D11/Balance_Sheet!D3</f>
         <v>0.1105</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="10">
         <f>Balance_Sheet!E11/Balance_Sheet!E3</f>
         <v>0.125094339622642</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="8">
+      <c r="B30" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="9">
         <f>365/(Balance_Sheet!D4/Ratios_Formulas!C14)</f>
         <v>103.199404761905</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="9">
         <f>365/(Balance_Sheet!E4/Ratios_Formulas!D14)</f>
         <v>105.288461538462</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="8">
+      <c r="B31" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="9">
         <f>365/(Balance_Sheet!D4/Ratios_Formulas!C15)</f>
         <v>83.6458333333333</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="9">
         <f>365/(Balance_Sheet!E4/Ratios_Formulas!D15)</f>
         <v>83.228021978022</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="8">
+      <c r="B32" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="9">
         <f>Balance_Sheet!D4/Ratios_Formulas!C18</f>
         <v>0.565203641526319</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="9">
         <f>Balance_Sheet!E4/Ratios_Formulas!D18</f>
         <v>0.558649786439237</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="8">
+      <c r="B33" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="9">
         <f>Balance_Sheet!D7/Balance_Sheet!D8</f>
         <v>6.66666666666667</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="9">
         <f>Balance_Sheet!E7/Balance_Sheet!E8</f>
         <v>7.53846153846154</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="8">
+      <c r="B34" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="9">
         <f>Balance_Sheet!D11/Ratios_Formulas!C7</f>
         <v>0.294666666666667</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="9">
         <f>Balance_Sheet!E11/Ratios_Formulas!D7</f>
         <v>0.368333333333333</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="8">
+      <c r="B35" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="9">
         <f>Balance_Sheet!I10/Ratios_Formulas!C7</f>
         <v>1.74708888888889</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="9">
         <f>Balance_Sheet!J10/Ratios_Formulas!D7</f>
         <v>1.98650555555556</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" s="8">
+      <c r="B36" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="9">
         <f>(C6*C7)/Balance_Sheet!D11</f>
         <v>16.9683257918552</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="9">
         <f>(D6*D7)/Balance_Sheet!E11</f>
         <v>13.5746606334842</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="B37" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="9">
         <f>(C6*C7)/Balance_Sheet!I10</f>
         <v>2.86190361108638</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="9">
         <f>(D6*D7)/Balance_Sheet!J10</f>
         <v>2.51698264120972</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="8">
+      <c r="B38" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="9">
         <f>(C6*C7+C9)/Balance_Sheet!D13</f>
         <v>10.3075416666667</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="9">
         <f>(D6*D7+D9)/Balance_Sheet!E13</f>
         <v>8.27956034482759</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="9">
+      <c r="B39" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="10">
         <f>C10/C6</f>
         <v>0.0206266666666667</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="10">
         <f>D10/D6</f>
         <v>0.0257833333333333</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>117</v>
+      <c r="E39" s="11" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="1"/>

</xml_diff>